<commit_message>
Add new model for encoder knob and changed code to work with latches
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -63,9 +63,6 @@
     <t>https://www.aliexpress.com/item/32842866575.html?spm=a2g0s.9042311.0.0.27424c4dpq9qo4</t>
   </si>
   <si>
-    <t>M2.5 x 8 Umbraco bolt</t>
-  </si>
-  <si>
     <t>M4 x 15 Umbraco bolt</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>5mm x 60mm smooth alu rod</t>
+  </si>
+  <si>
+    <t>M3 x 8 Umbraco bolt</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6" s="12">
         <v>16</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="12">
         <v>10</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="12">
         <v>8</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="12">
         <v>4</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="12">
         <v>4</v>
@@ -778,12 +778,12 @@
         <v>146</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="12">
         <v>4</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="12">
         <v>1</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="12">
         <v>8</v>
@@ -827,7 +827,7 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E10"/>
+    <hyperlink ref="E10" display="https://www.aliexpress.com/item/32613079212.html?spm=a2g0o.productlist.0.0.22ba3eb1qLseXx&amp;algo_pvid=a134bfe1-3b75-48a6-88eb-5a4ebeda4f22&amp;algo_expid=a134bfe1-3b75-48a6-88eb-5a4ebeda4f22-21&amp;btsid=842f2591-8817-4f0a-a82a-8665df723c52&amp;ws_ab_test=searchweb0_0,"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>